<commit_message>
[afin-dev] Integrated async functionality in conway_ops.onboarding for RepoSetup and ProjectCreator
</commit_message>
<xml_diff>
--- a/8002/EXPECTED@latest/Operator Reports/DevOps/Repo Stats.xlsx
+++ b/8002/EXPECTED@latest/Operator Reports/DevOps/Repo Stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\u2204-001\home\alex\consultant1@CCL\dev\conway_fork\conway.scenarios\8002\EXPECTED@latest\Operator Reports\DevOps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\u2204-001\home\alex\consultant1@CCL\dev\scratch_fork\scratch.scenarios\8002\EXPECTED@latest\Operator Reports\DevOps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7239E6B-578A-4F1A-B282-9E348FBEE24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF1F6C3-C463-4F01-B621-5C3E5B92B71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>